<commit_message>
requeter la base de donnee
</commit_message>
<xml_diff>
--- a/doc/BOT.xlsx
+++ b/doc/BOT.xlsx
@@ -14,9 +14,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>taux_it</t>
+  </si>
+  <si>
+    <t>var1</t>
+  </si>
+  <si>
+    <t>var2</t>
+  </si>
+  <si>
+    <t>var3</t>
+  </si>
+  <si>
+    <t>var4</t>
+  </si>
+  <si>
+    <t>var5</t>
+  </si>
+  <si>
+    <t>var6</t>
+  </si>
+  <si>
+    <t>var7</t>
+  </si>
+  <si>
+    <t>var8</t>
+  </si>
+  <si>
+    <t>var9</t>
+  </si>
+  <si>
+    <t>var10</t>
+  </si>
+  <si>
+    <t>var11</t>
+  </si>
+  <si>
+    <t>var12</t>
+  </si>
+  <si>
+    <t>var13</t>
+  </si>
+  <si>
+    <t>var14</t>
+  </si>
+  <si>
+    <t>var15</t>
+  </si>
+  <si>
+    <t>var16</t>
+  </si>
+  <si>
+    <t>var17</t>
+  </si>
+  <si>
+    <t>var18</t>
+  </si>
+  <si>
+    <t>var19</t>
+  </si>
+  <si>
+    <t>var20</t>
+  </si>
+  <si>
+    <t>var21</t>
+  </si>
+  <si>
+    <t>var22</t>
+  </si>
+  <si>
+    <t>var23</t>
+  </si>
+  <si>
+    <t>var24</t>
+  </si>
+  <si>
+    <t>var25</t>
+  </si>
+  <si>
+    <t>var26</t>
+  </si>
+  <si>
+    <t>var27</t>
+  </si>
+  <si>
+    <t>var28</t>
+  </si>
+  <si>
+    <t>var29</t>
+  </si>
+  <si>
+    <t>var30</t>
+  </si>
+  <si>
+    <t>var31</t>
+  </si>
+  <si>
+    <t>var32</t>
+  </si>
+  <si>
+    <t>var33</t>
+  </si>
+  <si>
+    <t>var34</t>
+  </si>
+  <si>
+    <t>var35</t>
+  </si>
+  <si>
+    <t>var36</t>
+  </si>
+  <si>
+    <t>var37</t>
+  </si>
+  <si>
+    <t>var38</t>
+  </si>
+  <si>
+    <t>var39</t>
+  </si>
+  <si>
+    <t>var40</t>
   </si>
 </sst>
 </file>
@@ -25,10 +145,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-* #,##0.0000000000_-;\-* #,##0.0000000000_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00000000000000000000000000_-;\-* #,##0.00000000000000000000000000_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00000000000000000000000000_-;\-* #,##0.00000000000000000000000000_-;_-* &quot;-&quot;??_-;_-@"/>
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -44,12 +164,12 @@
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Trebuchet MS"/>
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Trebuchet MS"/>
     </font>
   </fonts>
@@ -84,14 +204,16 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="168" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="168" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -318,125 +440,125 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F1" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="I1" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="J1" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="L1" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="O1" s="1">
-        <v>14.0</v>
-      </c>
-      <c r="P1" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="R1" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="S1" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="T1" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="U1" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="V1" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="W1" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="X1" s="1">
-        <v>23.0</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>29.0</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>32.0</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>34.0</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>35.0</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>36.0</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>37.0</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>38.0</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>39.0</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>40.0</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2">
@@ -939,25 +1061,18 @@
         <v>1488.5645836609692</v>
       </c>
     </row>
+    <row r="6" ht="1.5" customHeight="1"/>
     <row r="7">
-      <c r="B7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="T7" s="7">
-        <f>10000*T2</f>
-        <v>3222509.102</v>
-      </c>
+      <c r="C7" s="5"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8">
-      <c r="C8" s="8"/>
-      <c r="T8" s="9">
-        <v>0.05</v>
-      </c>
+      <c r="T8" s="7"/>
     </row>
-    <row r="9">
-      <c r="T9" s="7">
-        <f>95%*T7</f>
-        <v>3061383.647</v>
-      </c>
+    <row r="10">
+      <c r="B10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="T10" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>